<commit_message>
Added test cases for shoping cart.
</commit_message>
<xml_diff>
--- a/data/testplan.xlsx
+++ b/data/testplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="TS My address" sheetId="4" r:id="rId4"/>
     <sheet name="TS My wish list" sheetId="5" r:id="rId5"/>
     <sheet name="TS Personal Informations" sheetId="6" r:id="rId6"/>
+    <sheet name="TS Product cart" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="161">
   <si>
     <t>Scenarios</t>
   </si>
@@ -41,9 +42,6 @@
     <t>TS 3</t>
   </si>
   <si>
-    <t>TS 2</t>
-  </si>
-  <si>
     <t>TS 1</t>
   </si>
   <si>
@@ -131,18 +129,6 @@
     <t>ID: 6</t>
   </si>
   <si>
-    <t>Verify click on button "Order history and details"</t>
-  </si>
-  <si>
-    <t>Verify click on button "My credit slips"</t>
-  </si>
-  <si>
-    <t>Verifay click on button "My address"</t>
-  </si>
-  <si>
-    <t>Verify click on button "My personal information"</t>
-  </si>
-  <si>
     <t>MY ADDRESS</t>
   </si>
   <si>
@@ -152,9 +138,6 @@
     <t>MY WISH LIST</t>
   </si>
   <si>
-    <t>Verify click on button "My wish list"</t>
-  </si>
-  <si>
     <t>TS 5</t>
   </si>
   <si>
@@ -215,9 +198,6 @@
     <t>precondition</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>User data fields are displayed</t>
   </si>
   <si>
@@ -441,13 +421,100 @@
   </si>
   <si>
     <t>assert data</t>
+  </si>
+  <si>
+    <t>PRODUCT CART</t>
+  </si>
+  <si>
+    <t>Verify that user can add product in cart</t>
+  </si>
+  <si>
+    <t>Verify that user can add  product in cart quantity 3</t>
+  </si>
+  <si>
+    <t>Verify that user can add 3 products in cart</t>
+  </si>
+  <si>
+    <t>Verify that user can remove product from cart</t>
+  </si>
+  <si>
+    <t>TS 6</t>
+  </si>
+  <si>
+    <t>Click on button "Dresses"</t>
+  </si>
+  <si>
+    <t>Click on button "Add to cart" on first dress</t>
+  </si>
+  <si>
+    <t>Click on button "Procced to checkout</t>
+  </si>
+  <si>
+    <t>Your shopping cart contains: 1 Product</t>
+  </si>
+  <si>
+    <t>Click on button "Dresse"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is redirected on "Dresses" page </t>
+  </si>
+  <si>
+    <t>Click on button "Add to cart" on 1 dress</t>
+  </si>
+  <si>
+    <t>Click on button "Add to cart" on 2 dress</t>
+  </si>
+  <si>
+    <t>Click on button "Add to cart" on 3 dress</t>
+  </si>
+  <si>
+    <t>In field "Quantity" enter amount of products</t>
+  </si>
+  <si>
+    <t>New window appears with buttons "Continue shoping" and "Procced to checkout"</t>
+  </si>
+  <si>
+    <t>Click on button "Continue shoping"</t>
+  </si>
+  <si>
+    <t>Shoping page is displayed</t>
+  </si>
+  <si>
+    <t>ID: 4</t>
+  </si>
+  <si>
+    <t>Click on button "Cart"</t>
+  </si>
+  <si>
+    <t>New window appears with "SHOPPING-CART SUMMARY"</t>
+  </si>
+  <si>
+    <t>Your shopping cart contains: 2 Products</t>
+  </si>
+  <si>
+    <t>Click on button "Delete" in 1 product</t>
+  </si>
+  <si>
+    <t>Click on button "Delete" in 2 product</t>
+  </si>
+  <si>
+    <t>Click on button "Delete" in 3 product</t>
+  </si>
+  <si>
+    <t>Your shopping cart is empty.</t>
+  </si>
+  <si>
+    <t>Your shopping cart contains: 1 Product</t>
+  </si>
+  <si>
+    <t>Your shopping cart contains: 3 Products</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +538,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -480,7 +554,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -488,12 +562,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6D4D4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -523,6 +606,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -531,6 +617,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -812,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,7 +928,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -846,47 +945,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -895,68 +994,33 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -964,7 +1028,7 @@
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
@@ -972,7 +1036,7 @@
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -980,37 +1044,72 @@
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -1039,35 +1138,35 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1075,22 +1174,22 @@
     </row>
     <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1099,116 +1198,116 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D12" s="10" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1216,10 +1315,10 @@
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,54 +1326,54 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C28" s="8">
         <v>123456</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="D30" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1282,86 +1381,86 @@
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
         <v>87</v>
-      </c>
-      <c r="D36" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" t="s">
         <v>88</v>
-      </c>
-      <c r="D37" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D39" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D45" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1398,35 +1497,35 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1434,7 +1533,7 @@
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2"/>
     </row>
@@ -1450,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -1466,35 +1565,35 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1502,244 +1601,244 @@
     </row>
     <row r="3" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="14">
+        <v>61</v>
+      </c>
+      <c r="C25" s="15">
         <v>55000</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="14">
+        <v>64</v>
+      </c>
+      <c r="C26" s="15">
         <v>23456789</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D29" s="10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -1771,35 +1870,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1807,196 +1906,196 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2012,7 +2111,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2027,35 +2126,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -2063,85 +2162,85 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>125</v>
+        <v>113</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2154,4 +2253,285 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="39.88671875" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.21875" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>